<commit_message>
Remove old Colab notebook and reorganize mock databases
</commit_message>
<xml_diff>
--- a/input/mock_databases/Power_Query_Database_mock.xlsx
+++ b/input/mock_databases/Power_Query_Database_mock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g/Documents/pdf_form_filler/input/mock_databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D22CC8-F8B4-EF40-9985-21D94B3CFDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63D2AEC-CC97-3249-A889-4C99D44B5E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="10660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PQ_DATABASE" sheetId="3" r:id="rId1"/>
@@ -14647,8 +14647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>